<commit_message>
aggiunta una colonna nella tabella
</commit_message>
<xml_diff>
--- a/input_signal_table.xlsx
+++ b/input_signal_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carloradice\Documents\IILTSpice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D79E7A92-F025-4FB3-9F1A-2BC416FE350A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A260639-05E2-4989-BFCC-27D8437520A1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>A1</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>Totale in decimale</t>
+  </si>
+  <si>
+    <t>Totale in binario</t>
   </si>
 </sst>
 </file>
@@ -86,14 +89,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -120,19 +130,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{ABC6E893-DB51-4D88-B945-8B3554FC614D}" name="Tabella4" displayName="Tabella4" ref="B1:I17" totalsRowShown="0">
-  <autoFilter ref="B1:I17" xr:uid="{F142AE51-C037-45D6-9B41-496128C10C66}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{ABC6E893-DB51-4D88-B945-8B3554FC614D}" name="Tabella4" displayName="Tabella4" ref="B1:J17" totalsRowShown="0">
+  <autoFilter ref="B1:J17" xr:uid="{F142AE51-C037-45D6-9B41-496128C10C66}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{D2993595-EAFA-4A13-92BA-12D4F842A9A0}" name="A1"/>
     <tableColumn id="2" xr3:uid="{52025968-B10A-47F5-8C31-5D0A1F82318E}" name="A0"/>
     <tableColumn id="3" xr3:uid="{178E1EA7-345C-46C6-9F3E-A5D84B13FAF6}" name="B1"/>
     <tableColumn id="4" xr3:uid="{1D40A5E1-8D85-4D88-B87B-68F133423B58}" name="B0"/>
-    <tableColumn id="5" xr3:uid="{11CD62CD-F15D-4596-AE64-799DA157B45B}" name="Carry Out" dataDxfId="1">
+    <tableColumn id="5" xr3:uid="{11CD62CD-F15D-4596-AE64-799DA157B45B}" name="Carry Out" dataDxfId="3">
       <calculatedColumnFormula>_xludf.MID(Tabella4[[#This Row],[Totale in decimale]], _xludf.COLUMN()-(_xludf.COLUMN(Tabella4[[#This Row],[Carry Out]]) -1), 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{485AB37F-7006-48C5-9087-826B2F9BC2E4}" name="Y1" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{485AB37F-7006-48C5-9087-826B2F9BC2E4}" name="Y1" dataDxfId="4"/>
     <tableColumn id="7" xr3:uid="{9CF4FF90-FC88-4FA1-9000-6AAA392C9373}" name="Y0" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{C0F7D211-AA4E-4C30-97D4-BB2821247A6E}" name="Totale in decimale" dataDxfId="0">
+    <tableColumn id="9" xr3:uid="{ABF6D987-3AC0-46F3-AA62-34B6B58D3DE1}" name="Totale in binario" dataDxfId="0">
+      <calculatedColumnFormula>DEC2BIN(SUM(SUM(PRODUCT(Tabella4[[#This Row],[A1]]*2) + (PRODUCT(Tabella4[[#This Row],[A0]] * 1))) + SUM(PRODUCT(Tabella4[[#This Row],[B1]]*2) + (PRODUCT(Tabella4[[#This Row],[B0]] * 1)))))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{C0F7D211-AA4E-4C30-97D4-BB2821247A6E}" name="Totale in decimale" dataDxfId="1">
       <calculatedColumnFormula>(SUM(SUM(PRODUCT(Tabella4[[#This Row],[A1]]*2) + (PRODUCT(Tabella4[[#This Row],[A0]] * 1))) + SUM(PRODUCT(Tabella4[[#This Row],[B1]]*2) + (PRODUCT(Tabella4[[#This Row],[B0]] * 1)))))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -437,20 +450,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:I17"/>
+  <dimension ref="B1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.6640625" customWidth="1"/>
-    <col min="9" max="9" width="18.88671875" customWidth="1"/>
+    <col min="9" max="9" width="17.21875" customWidth="1"/>
+    <col min="10" max="10" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -473,10 +487,13 @@
         <v>6</v>
       </c>
       <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>0</v>
       </c>
@@ -498,12 +515,16 @@
       <c r="H2" s="1">
         <v>0</v>
       </c>
-      <c r="I2" s="1">
-        <f>(SUM(SUM(PRODUCT(Tabella4[[#This Row],[A1]]*2) + (PRODUCT(Tabella4[[#This Row],[A0]] * 1))) + SUM(PRODUCT(Tabella4[[#This Row],[B1]]*2) + (PRODUCT(Tabella4[[#This Row],[B0]] * 1)))))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I2" s="2" t="str">
+        <f>DEC2BIN(SUM(SUM(PRODUCT(Tabella4[[#This Row],[A1]]*2) + (PRODUCT(Tabella4[[#This Row],[A0]] * 1))) + SUM(PRODUCT(Tabella4[[#This Row],[B1]]*2) + (PRODUCT(Tabella4[[#This Row],[B0]] * 1)))))</f>
+        <v>0</v>
+      </c>
+      <c r="J2" s="1">
+        <f>(SUM(SUM(PRODUCT(Tabella4[[#This Row],[A1]]*2) + (PRODUCT(Tabella4[[#This Row],[A0]] * 1))) + SUM(PRODUCT(Tabella4[[#This Row],[B1]]*2) + (PRODUCT(Tabella4[[#This Row],[B0]] * 1)))))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>0</v>
       </c>
@@ -525,12 +546,16 @@
       <c r="H3" s="1">
         <v>1</v>
       </c>
-      <c r="I3" s="1">
-        <f>(SUM(SUM(PRODUCT(Tabella4[[#This Row],[A1]]*2) + (PRODUCT(Tabella4[[#This Row],[A0]] * 1))) + SUM(PRODUCT(Tabella4[[#This Row],[B1]]*2) + (PRODUCT(Tabella4[[#This Row],[B0]] * 1)))))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I3" s="2" t="str">
+        <f>DEC2BIN(SUM(SUM(PRODUCT(Tabella4[[#This Row],[A1]]*2) + (PRODUCT(Tabella4[[#This Row],[A0]] * 1))) + SUM(PRODUCT(Tabella4[[#This Row],[B1]]*2) + (PRODUCT(Tabella4[[#This Row],[B0]] * 1)))))</f>
+        <v>1</v>
+      </c>
+      <c r="J3" s="1">
+        <f>(SUM(SUM(PRODUCT(Tabella4[[#This Row],[A1]]*2) + (PRODUCT(Tabella4[[#This Row],[A0]] * 1))) + SUM(PRODUCT(Tabella4[[#This Row],[B1]]*2) + (PRODUCT(Tabella4[[#This Row],[B0]] * 1)))))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>0</v>
       </c>
@@ -552,12 +577,16 @@
       <c r="H4" s="1">
         <v>0</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="2" t="str">
+        <f>DEC2BIN(SUM(SUM(PRODUCT(Tabella4[[#This Row],[A1]]*2) + (PRODUCT(Tabella4[[#This Row],[A0]] * 1))) + SUM(PRODUCT(Tabella4[[#This Row],[B1]]*2) + (PRODUCT(Tabella4[[#This Row],[B0]] * 1)))))</f>
+        <v>10</v>
+      </c>
+      <c r="J4" s="1">
         <f>(SUM(SUM(PRODUCT(Tabella4[[#This Row],[A1]]*2) + (PRODUCT(Tabella4[[#This Row],[A0]] * 1))) + SUM(PRODUCT(Tabella4[[#This Row],[B1]]*2) + (PRODUCT(Tabella4[[#This Row],[B0]] * 1)))))</f>
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>0</v>
       </c>
@@ -579,12 +608,16 @@
       <c r="H5" s="1">
         <v>1</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I5" s="2" t="str">
+        <f>DEC2BIN(SUM(SUM(PRODUCT(Tabella4[[#This Row],[A1]]*2) + (PRODUCT(Tabella4[[#This Row],[A0]] * 1))) + SUM(PRODUCT(Tabella4[[#This Row],[B1]]*2) + (PRODUCT(Tabella4[[#This Row],[B0]] * 1)))))</f>
+        <v>11</v>
+      </c>
+      <c r="J5" s="1">
         <f>(SUM(SUM(PRODUCT(Tabella4[[#This Row],[A1]]*2) + (PRODUCT(Tabella4[[#This Row],[A0]] * 1))) + SUM(PRODUCT(Tabella4[[#This Row],[B1]]*2) + (PRODUCT(Tabella4[[#This Row],[B0]] * 1)))))</f>
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>0</v>
       </c>
@@ -606,12 +639,16 @@
       <c r="H6" s="1">
         <v>1</v>
       </c>
-      <c r="I6" s="1">
-        <f>(SUM(SUM(PRODUCT(Tabella4[[#This Row],[A1]]*2) + (PRODUCT(Tabella4[[#This Row],[A0]] * 1))) + SUM(PRODUCT(Tabella4[[#This Row],[B1]]*2) + (PRODUCT(Tabella4[[#This Row],[B0]] * 1)))))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I6" s="2" t="str">
+        <f>DEC2BIN(SUM(SUM(PRODUCT(Tabella4[[#This Row],[A1]]*2) + (PRODUCT(Tabella4[[#This Row],[A0]] * 1))) + SUM(PRODUCT(Tabella4[[#This Row],[B1]]*2) + (PRODUCT(Tabella4[[#This Row],[B0]] * 1)))))</f>
+        <v>1</v>
+      </c>
+      <c r="J6" s="1">
+        <f>(SUM(SUM(PRODUCT(Tabella4[[#This Row],[A1]]*2) + (PRODUCT(Tabella4[[#This Row],[A0]] * 1))) + SUM(PRODUCT(Tabella4[[#This Row],[B1]]*2) + (PRODUCT(Tabella4[[#This Row],[B0]] * 1)))))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>0</v>
       </c>
@@ -633,12 +670,16 @@
       <c r="H7" s="1">
         <v>0</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="2" t="str">
+        <f>DEC2BIN(SUM(SUM(PRODUCT(Tabella4[[#This Row],[A1]]*2) + (PRODUCT(Tabella4[[#This Row],[A0]] * 1))) + SUM(PRODUCT(Tabella4[[#This Row],[B1]]*2) + (PRODUCT(Tabella4[[#This Row],[B0]] * 1)))))</f>
+        <v>10</v>
+      </c>
+      <c r="J7" s="1">
         <f>(SUM(SUM(PRODUCT(Tabella4[[#This Row],[A1]]*2) + (PRODUCT(Tabella4[[#This Row],[A0]] * 1))) + SUM(PRODUCT(Tabella4[[#This Row],[B1]]*2) + (PRODUCT(Tabella4[[#This Row],[B0]] * 1)))))</f>
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>0</v>
       </c>
@@ -660,12 +701,16 @@
       <c r="H8" s="1">
         <v>1</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8" s="2" t="str">
+        <f>DEC2BIN(SUM(SUM(PRODUCT(Tabella4[[#This Row],[A1]]*2) + (PRODUCT(Tabella4[[#This Row],[A0]] * 1))) + SUM(PRODUCT(Tabella4[[#This Row],[B1]]*2) + (PRODUCT(Tabella4[[#This Row],[B0]] * 1)))))</f>
+        <v>11</v>
+      </c>
+      <c r="J8" s="1">
         <f>(SUM(SUM(PRODUCT(Tabella4[[#This Row],[A1]]*2) + (PRODUCT(Tabella4[[#This Row],[A0]] * 1))) + SUM(PRODUCT(Tabella4[[#This Row],[B1]]*2) + (PRODUCT(Tabella4[[#This Row],[B0]] * 1)))))</f>
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>0</v>
       </c>
@@ -687,12 +732,16 @@
       <c r="H9" s="1">
         <v>0</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I9" s="2" t="str">
+        <f>DEC2BIN(SUM(SUM(PRODUCT(Tabella4[[#This Row],[A1]]*2) + (PRODUCT(Tabella4[[#This Row],[A0]] * 1))) + SUM(PRODUCT(Tabella4[[#This Row],[B1]]*2) + (PRODUCT(Tabella4[[#This Row],[B0]] * 1)))))</f>
+        <v>100</v>
+      </c>
+      <c r="J9" s="1">
         <f>(SUM(SUM(PRODUCT(Tabella4[[#This Row],[A1]]*2) + (PRODUCT(Tabella4[[#This Row],[A0]] * 1))) + SUM(PRODUCT(Tabella4[[#This Row],[B1]]*2) + (PRODUCT(Tabella4[[#This Row],[B0]] * 1)))))</f>
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>1</v>
       </c>
@@ -714,12 +763,16 @@
       <c r="H10" s="1">
         <v>0</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I10" s="2" t="str">
+        <f>DEC2BIN(SUM(SUM(PRODUCT(Tabella4[[#This Row],[A1]]*2) + (PRODUCT(Tabella4[[#This Row],[A0]] * 1))) + SUM(PRODUCT(Tabella4[[#This Row],[B1]]*2) + (PRODUCT(Tabella4[[#This Row],[B0]] * 1)))))</f>
+        <v>10</v>
+      </c>
+      <c r="J10" s="1">
         <f>(SUM(SUM(PRODUCT(Tabella4[[#This Row],[A1]]*2) + (PRODUCT(Tabella4[[#This Row],[A0]] * 1))) + SUM(PRODUCT(Tabella4[[#This Row],[B1]]*2) + (PRODUCT(Tabella4[[#This Row],[B0]] * 1)))))</f>
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>1</v>
       </c>
@@ -741,12 +794,16 @@
       <c r="H11" s="1">
         <v>1</v>
       </c>
-      <c r="I11" s="1">
+      <c r="I11" s="2" t="str">
+        <f>DEC2BIN(SUM(SUM(PRODUCT(Tabella4[[#This Row],[A1]]*2) + (PRODUCT(Tabella4[[#This Row],[A0]] * 1))) + SUM(PRODUCT(Tabella4[[#This Row],[B1]]*2) + (PRODUCT(Tabella4[[#This Row],[B0]] * 1)))))</f>
+        <v>11</v>
+      </c>
+      <c r="J11" s="1">
         <f>(SUM(SUM(PRODUCT(Tabella4[[#This Row],[A1]]*2) + (PRODUCT(Tabella4[[#This Row],[A0]] * 1))) + SUM(PRODUCT(Tabella4[[#This Row],[B1]]*2) + (PRODUCT(Tabella4[[#This Row],[B0]] * 1)))))</f>
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>1</v>
       </c>
@@ -768,12 +825,16 @@
       <c r="H12" s="1">
         <v>0</v>
       </c>
-      <c r="I12" s="1">
+      <c r="I12" s="2" t="str">
+        <f>DEC2BIN(SUM(SUM(PRODUCT(Tabella4[[#This Row],[A1]]*2) + (PRODUCT(Tabella4[[#This Row],[A0]] * 1))) + SUM(PRODUCT(Tabella4[[#This Row],[B1]]*2) + (PRODUCT(Tabella4[[#This Row],[B0]] * 1)))))</f>
+        <v>100</v>
+      </c>
+      <c r="J12" s="1">
         <f>(SUM(SUM(PRODUCT(Tabella4[[#This Row],[A1]]*2) + (PRODUCT(Tabella4[[#This Row],[A0]] * 1))) + SUM(PRODUCT(Tabella4[[#This Row],[B1]]*2) + (PRODUCT(Tabella4[[#This Row],[B0]] * 1)))))</f>
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>1</v>
       </c>
@@ -795,12 +856,16 @@
       <c r="H13" s="1">
         <v>1</v>
       </c>
-      <c r="I13" s="1">
+      <c r="I13" s="2" t="str">
+        <f>DEC2BIN(SUM(SUM(PRODUCT(Tabella4[[#This Row],[A1]]*2) + (PRODUCT(Tabella4[[#This Row],[A0]] * 1))) + SUM(PRODUCT(Tabella4[[#This Row],[B1]]*2) + (PRODUCT(Tabella4[[#This Row],[B0]] * 1)))))</f>
+        <v>101</v>
+      </c>
+      <c r="J13" s="1">
         <f>(SUM(SUM(PRODUCT(Tabella4[[#This Row],[A1]]*2) + (PRODUCT(Tabella4[[#This Row],[A0]] * 1))) + SUM(PRODUCT(Tabella4[[#This Row],[B1]]*2) + (PRODUCT(Tabella4[[#This Row],[B0]] * 1)))))</f>
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>1</v>
       </c>
@@ -822,12 +887,16 @@
       <c r="H14" s="1">
         <v>1</v>
       </c>
-      <c r="I14" s="1">
+      <c r="I14" s="2" t="str">
+        <f>DEC2BIN(SUM(SUM(PRODUCT(Tabella4[[#This Row],[A1]]*2) + (PRODUCT(Tabella4[[#This Row],[A0]] * 1))) + SUM(PRODUCT(Tabella4[[#This Row],[B1]]*2) + (PRODUCT(Tabella4[[#This Row],[B0]] * 1)))))</f>
+        <v>11</v>
+      </c>
+      <c r="J14" s="1">
         <f>(SUM(SUM(PRODUCT(Tabella4[[#This Row],[A1]]*2) + (PRODUCT(Tabella4[[#This Row],[A0]] * 1))) + SUM(PRODUCT(Tabella4[[#This Row],[B1]]*2) + (PRODUCT(Tabella4[[#This Row],[B0]] * 1)))))</f>
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>1</v>
       </c>
@@ -849,12 +918,16 @@
       <c r="H15" s="1">
         <v>0</v>
       </c>
-      <c r="I15" s="1">
+      <c r="I15" s="2" t="str">
+        <f>DEC2BIN(SUM(SUM(PRODUCT(Tabella4[[#This Row],[A1]]*2) + (PRODUCT(Tabella4[[#This Row],[A0]] * 1))) + SUM(PRODUCT(Tabella4[[#This Row],[B1]]*2) + (PRODUCT(Tabella4[[#This Row],[B0]] * 1)))))</f>
+        <v>100</v>
+      </c>
+      <c r="J15" s="1">
         <f>(SUM(SUM(PRODUCT(Tabella4[[#This Row],[A1]]*2) + (PRODUCT(Tabella4[[#This Row],[A0]] * 1))) + SUM(PRODUCT(Tabella4[[#This Row],[B1]]*2) + (PRODUCT(Tabella4[[#This Row],[B0]] * 1)))))</f>
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>1</v>
       </c>
@@ -876,12 +949,16 @@
       <c r="H16" s="1">
         <v>1</v>
       </c>
-      <c r="I16" s="1">
+      <c r="I16" s="2" t="str">
+        <f>DEC2BIN(SUM(SUM(PRODUCT(Tabella4[[#This Row],[A1]]*2) + (PRODUCT(Tabella4[[#This Row],[A0]] * 1))) + SUM(PRODUCT(Tabella4[[#This Row],[B1]]*2) + (PRODUCT(Tabella4[[#This Row],[B0]] * 1)))))</f>
+        <v>101</v>
+      </c>
+      <c r="J16" s="1">
         <f>(SUM(SUM(PRODUCT(Tabella4[[#This Row],[A1]]*2) + (PRODUCT(Tabella4[[#This Row],[A0]] * 1))) + SUM(PRODUCT(Tabella4[[#This Row],[B1]]*2) + (PRODUCT(Tabella4[[#This Row],[B0]] * 1)))))</f>
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>1</v>
       </c>
@@ -903,7 +980,11 @@
       <c r="H17" s="1">
         <v>0</v>
       </c>
-      <c r="I17" s="1">
+      <c r="I17" s="2" t="str">
+        <f>DEC2BIN(SUM(SUM(PRODUCT(Tabella4[[#This Row],[A1]]*2) + (PRODUCT(Tabella4[[#This Row],[A0]] * 1))) + SUM(PRODUCT(Tabella4[[#This Row],[B1]]*2) + (PRODUCT(Tabella4[[#This Row],[B0]] * 1)))))</f>
+        <v>110</v>
+      </c>
+      <c r="J17" s="1">
         <f>(SUM(SUM(PRODUCT(Tabella4[[#This Row],[A1]]*2) + (PRODUCT(Tabella4[[#This Row],[A0]] * 1))) + SUM(PRODUCT(Tabella4[[#This Row],[B1]]*2) + (PRODUCT(Tabella4[[#This Row],[B0]] * 1)))))</f>
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
aggiunta schematica del multiplexer 1x2 necessario per usare l'ENABLE con i registri. Modificato lo schema dei registri che ora hanno anche i multiplexer prima del D-flip-flop. Rimossi i plot perchè sbagliati, creata la cartella per organizzare i plot futuri
</commit_message>
<xml_diff>
--- a/input_signal_table.xlsx
+++ b/input_signal_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carloradice\Documents\IILTSpice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A260639-05E2-4989-BFCC-27D8437520A1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52911251-9614-42A6-A1AE-793E7339D096}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>A1</t>
   </si>
@@ -55,12 +55,42 @@
   <si>
     <t>Totale in binario</t>
   </si>
+  <si>
+    <t>RESET</t>
+  </si>
+  <si>
+    <t>PRESET</t>
+  </si>
+  <si>
+    <t>ENABLE</t>
+  </si>
+  <si>
+    <t>I1</t>
+  </si>
+  <si>
+    <t>I2</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>Se ENABLE = 0 stato HOLD</t>
+  </si>
+  <si>
+    <t>RESET = 1</t>
+  </si>
+  <si>
+    <t>PRESET = 1</t>
+  </si>
+  <si>
+    <t>Non può accadere che RESET e PRESET siano entrambi a 1 o che RESET o PRESET = 1 quando ENABLE = 0</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,13 +98,45 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -89,12 +151,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -102,10 +174,10 @@
   <dxfs count="5">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -137,17 +209,33 @@
     <tableColumn id="2" xr3:uid="{52025968-B10A-47F5-8C31-5D0A1F82318E}" name="A0"/>
     <tableColumn id="3" xr3:uid="{178E1EA7-345C-46C6-9F3E-A5D84B13FAF6}" name="B1"/>
     <tableColumn id="4" xr3:uid="{1D40A5E1-8D85-4D88-B87B-68F133423B58}" name="B0"/>
-    <tableColumn id="5" xr3:uid="{11CD62CD-F15D-4596-AE64-799DA157B45B}" name="Carry Out" dataDxfId="3">
+    <tableColumn id="5" xr3:uid="{11CD62CD-F15D-4596-AE64-799DA157B45B}" name="Carry Out" dataDxfId="4">
       <calculatedColumnFormula>_xludf.MID(Tabella4[[#This Row],[Totale in decimale]], _xludf.COLUMN()-(_xludf.COLUMN(Tabella4[[#This Row],[Carry Out]]) -1), 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{485AB37F-7006-48C5-9087-826B2F9BC2E4}" name="Y1" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{485AB37F-7006-48C5-9087-826B2F9BC2E4}" name="Y1" dataDxfId="3"/>
     <tableColumn id="7" xr3:uid="{9CF4FF90-FC88-4FA1-9000-6AAA392C9373}" name="Y0" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{ABF6D987-3AC0-46F3-AA62-34B6B58D3DE1}" name="Totale in binario" dataDxfId="0">
+    <tableColumn id="9" xr3:uid="{ABF6D987-3AC0-46F3-AA62-34B6B58D3DE1}" name="Totale in binario" dataDxfId="1">
       <calculatedColumnFormula>DEC2BIN(SUM(SUM(PRODUCT(Tabella4[[#This Row],[A1]]*2) + (PRODUCT(Tabella4[[#This Row],[A0]] * 1))) + SUM(PRODUCT(Tabella4[[#This Row],[B1]]*2) + (PRODUCT(Tabella4[[#This Row],[B0]] * 1)))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C0F7D211-AA4E-4C30-97D4-BB2821247A6E}" name="Totale in decimale" dataDxfId="1">
+    <tableColumn id="8" xr3:uid="{C0F7D211-AA4E-4C30-97D4-BB2821247A6E}" name="Totale in decimale" dataDxfId="0">
       <calculatedColumnFormula>(SUM(SUM(PRODUCT(Tabella4[[#This Row],[A1]]*2) + (PRODUCT(Tabella4[[#This Row],[A0]] * 1))) + SUM(PRODUCT(Tabella4[[#This Row],[B1]]*2) + (PRODUCT(Tabella4[[#This Row],[B0]] * 1)))))</calculatedColumnFormula>
     </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F0BD78C1-F0EE-450D-A251-57E4EA9297B9}" name="Tabella1" displayName="Tabella1" ref="B20:H52" totalsRowShown="0">
+  <autoFilter ref="B20:H52" xr:uid="{FA68169B-2A3F-4DD9-8590-32826CC5A2B8}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{0C2D47DF-5F36-4A6E-A369-C37FC2452565}" name="I1"/>
+    <tableColumn id="2" xr3:uid="{5DDB4E52-E688-4863-B530-2D8BD3BE24A8}" name="I2"/>
+    <tableColumn id="3" xr3:uid="{DE535522-D472-4317-AAFE-898B4902263C}" name="RESET"/>
+    <tableColumn id="4" xr3:uid="{50723725-C12B-4A0A-A084-23474A44855E}" name="PRESET"/>
+    <tableColumn id="5" xr3:uid="{46212E3D-E1E1-4EC6-B50A-8E9082C10C99}" name="ENABLE"/>
+    <tableColumn id="6" xr3:uid="{DF40D4E5-1D56-4C64-B848-CB9206012036}" name="A1"/>
+    <tableColumn id="7" xr3:uid="{AD2DAE48-85BC-46DE-97F7-2D2C8DF806AC}" name="A2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -450,16 +538,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:J17"/>
+  <dimension ref="A1:R88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="J59" sqref="J59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.6640625" customWidth="1"/>
+    <col min="7" max="8" width="10.88671875" customWidth="1"/>
     <col min="9" max="9" width="17.21875" customWidth="1"/>
     <col min="10" max="10" width="19.44140625" customWidth="1"/>
   </cols>
@@ -958,7 +1047,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>1</v>
       </c>
@@ -989,13 +1078,1113 @@
         <v>6</v>
       </c>
     </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" t="s">
+        <v>0</v>
+      </c>
+      <c r="H20" t="s">
+        <v>14</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21" s="4">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K21" s="4"/>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22" s="5">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B23" s="3">
+        <v>0</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0</v>
+      </c>
+      <c r="E23" s="3">
+        <v>1</v>
+      </c>
+      <c r="F23" s="3">
+        <v>0</v>
+      </c>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="J23" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24" s="7">
+        <v>1</v>
+      </c>
+      <c r="F24" s="5">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B25" s="3">
+        <v>0</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0</v>
+      </c>
+      <c r="D25" s="3">
+        <v>1</v>
+      </c>
+      <c r="E25" s="3">
+        <v>0</v>
+      </c>
+      <c r="F25" s="3">
+        <v>0</v>
+      </c>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26" s="6">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" s="5">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B27" s="3">
+        <v>0</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0</v>
+      </c>
+      <c r="D27" s="3">
+        <v>1</v>
+      </c>
+      <c r="E27" s="3">
+        <v>1</v>
+      </c>
+      <c r="F27" s="3">
+        <v>0</v>
+      </c>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+    </row>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B28" s="3">
+        <v>0</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0</v>
+      </c>
+      <c r="D28" s="3">
+        <v>1</v>
+      </c>
+      <c r="E28" s="3">
+        <v>1</v>
+      </c>
+      <c r="F28" s="3">
+        <v>1</v>
+      </c>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+    </row>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29" s="4">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30" s="5">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B31" s="3">
+        <v>0</v>
+      </c>
+      <c r="C31" s="3">
+        <v>1</v>
+      </c>
+      <c r="D31" s="3">
+        <v>0</v>
+      </c>
+      <c r="E31" s="3">
+        <v>1</v>
+      </c>
+      <c r="F31" s="3">
+        <v>0</v>
+      </c>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32" s="7">
+        <v>1</v>
+      </c>
+      <c r="F32" s="5">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="5"/>
+      <c r="B33" s="3">
+        <v>0</v>
+      </c>
+      <c r="C33" s="3">
+        <v>1</v>
+      </c>
+      <c r="D33" s="3">
+        <v>1</v>
+      </c>
+      <c r="E33" s="3">
+        <v>0</v>
+      </c>
+      <c r="F33" s="3">
+        <v>0</v>
+      </c>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="5"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="5"/>
+      <c r="B34" s="5">
+        <v>0</v>
+      </c>
+      <c r="C34" s="5">
+        <v>1</v>
+      </c>
+      <c r="D34" s="6">
+        <v>1</v>
+      </c>
+      <c r="E34" s="5">
+        <v>0</v>
+      </c>
+      <c r="F34" s="5">
+        <v>1</v>
+      </c>
+      <c r="G34" s="5">
+        <v>0</v>
+      </c>
+      <c r="H34" s="5">
+        <v>1</v>
+      </c>
+      <c r="I34" s="5"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="5"/>
+      <c r="B35" s="3">
+        <v>0</v>
+      </c>
+      <c r="C35" s="3">
+        <v>1</v>
+      </c>
+      <c r="D35" s="3">
+        <v>1</v>
+      </c>
+      <c r="E35" s="3">
+        <v>1</v>
+      </c>
+      <c r="F35" s="3">
+        <v>0</v>
+      </c>
+      <c r="G35" s="3"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="5"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="5"/>
+      <c r="B36" s="3">
+        <v>0</v>
+      </c>
+      <c r="C36" s="3">
+        <v>1</v>
+      </c>
+      <c r="D36" s="3">
+        <v>1</v>
+      </c>
+      <c r="E36" s="3">
+        <v>1</v>
+      </c>
+      <c r="F36" s="3">
+        <v>1</v>
+      </c>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="5"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="5"/>
+      <c r="B37" s="5">
+        <v>1</v>
+      </c>
+      <c r="C37" s="5">
+        <v>0</v>
+      </c>
+      <c r="D37" s="5">
+        <v>0</v>
+      </c>
+      <c r="E37" s="5">
+        <v>0</v>
+      </c>
+      <c r="F37" s="4">
+        <v>0</v>
+      </c>
+      <c r="G37" s="5">
+        <v>1</v>
+      </c>
+      <c r="H37" s="5">
+        <v>0</v>
+      </c>
+      <c r="I37" s="5"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="5"/>
+      <c r="B38" s="5">
+        <v>1</v>
+      </c>
+      <c r="C38" s="5">
+        <v>0</v>
+      </c>
+      <c r="D38" s="5">
+        <v>0</v>
+      </c>
+      <c r="E38" s="5">
+        <v>0</v>
+      </c>
+      <c r="F38" s="5">
+        <v>1</v>
+      </c>
+      <c r="G38" s="5">
+        <v>1</v>
+      </c>
+      <c r="H38" s="5">
+        <v>0</v>
+      </c>
+      <c r="I38" s="5"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="5"/>
+      <c r="B39" s="3">
+        <v>1</v>
+      </c>
+      <c r="C39" s="3">
+        <v>0</v>
+      </c>
+      <c r="D39" s="3">
+        <v>0</v>
+      </c>
+      <c r="E39" s="3">
+        <v>1</v>
+      </c>
+      <c r="F39" s="3">
+        <v>0</v>
+      </c>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="5"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" s="5"/>
+      <c r="B40" s="5">
+        <v>1</v>
+      </c>
+      <c r="C40" s="5">
+        <v>0</v>
+      </c>
+      <c r="D40" s="5">
+        <v>0</v>
+      </c>
+      <c r="E40" s="7">
+        <v>1</v>
+      </c>
+      <c r="F40" s="5">
+        <v>1</v>
+      </c>
+      <c r="G40" s="5">
+        <v>1</v>
+      </c>
+      <c r="H40" s="5">
+        <v>1</v>
+      </c>
+      <c r="I40" s="5"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" s="5"/>
+      <c r="B41" s="3">
+        <v>1</v>
+      </c>
+      <c r="C41" s="3">
+        <v>0</v>
+      </c>
+      <c r="D41" s="3">
+        <v>1</v>
+      </c>
+      <c r="E41" s="3">
+        <v>0</v>
+      </c>
+      <c r="F41" s="3">
+        <v>0</v>
+      </c>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="5"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" s="5"/>
+      <c r="B42" s="5">
+        <v>1</v>
+      </c>
+      <c r="C42" s="5">
+        <v>0</v>
+      </c>
+      <c r="D42" s="6">
+        <v>1</v>
+      </c>
+      <c r="E42" s="5">
+        <v>0</v>
+      </c>
+      <c r="F42" s="5">
+        <v>1</v>
+      </c>
+      <c r="G42" s="5">
+        <v>0</v>
+      </c>
+      <c r="H42" s="5">
+        <v>0</v>
+      </c>
+      <c r="I42" s="5"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" s="5"/>
+      <c r="B43" s="3">
+        <v>1</v>
+      </c>
+      <c r="C43" s="3">
+        <v>0</v>
+      </c>
+      <c r="D43" s="3">
+        <v>1</v>
+      </c>
+      <c r="E43" s="3">
+        <v>1</v>
+      </c>
+      <c r="F43" s="3">
+        <v>0</v>
+      </c>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="5"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" s="5"/>
+      <c r="B44" s="3">
+        <v>1</v>
+      </c>
+      <c r="C44" s="3">
+        <v>0</v>
+      </c>
+      <c r="D44" s="3">
+        <v>1</v>
+      </c>
+      <c r="E44" s="3">
+        <v>1</v>
+      </c>
+      <c r="F44" s="3">
+        <v>1</v>
+      </c>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="5"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" s="5"/>
+      <c r="B45" s="5">
+        <v>1</v>
+      </c>
+      <c r="C45" s="5">
+        <v>1</v>
+      </c>
+      <c r="D45" s="5">
+        <v>0</v>
+      </c>
+      <c r="E45" s="5">
+        <v>0</v>
+      </c>
+      <c r="F45" s="4">
+        <v>0</v>
+      </c>
+      <c r="G45" s="5">
+        <v>1</v>
+      </c>
+      <c r="H45" s="5">
+        <v>1</v>
+      </c>
+      <c r="I45" s="5"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46" s="5"/>
+      <c r="B46" s="5">
+        <v>1</v>
+      </c>
+      <c r="C46" s="5">
+        <v>1</v>
+      </c>
+      <c r="D46" s="5">
+        <v>0</v>
+      </c>
+      <c r="E46" s="5">
+        <v>0</v>
+      </c>
+      <c r="F46" s="5">
+        <v>1</v>
+      </c>
+      <c r="G46" s="5">
+        <v>1</v>
+      </c>
+      <c r="H46" s="5">
+        <v>1</v>
+      </c>
+      <c r="I46" s="5"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47" s="5"/>
+      <c r="B47" s="3">
+        <v>1</v>
+      </c>
+      <c r="C47" s="3">
+        <v>1</v>
+      </c>
+      <c r="D47" s="3">
+        <v>0</v>
+      </c>
+      <c r="E47" s="3">
+        <v>1</v>
+      </c>
+      <c r="F47" s="3">
+        <v>0</v>
+      </c>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="5"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48" s="5"/>
+      <c r="B48" s="5">
+        <v>1</v>
+      </c>
+      <c r="C48" s="5">
+        <v>1</v>
+      </c>
+      <c r="D48" s="5">
+        <v>0</v>
+      </c>
+      <c r="E48" s="7">
+        <v>1</v>
+      </c>
+      <c r="F48" s="5">
+        <v>1</v>
+      </c>
+      <c r="G48" s="5">
+        <v>1</v>
+      </c>
+      <c r="H48" s="5">
+        <v>1</v>
+      </c>
+      <c r="I48" s="5"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" s="5"/>
+      <c r="B49" s="3">
+        <v>1</v>
+      </c>
+      <c r="C49" s="3">
+        <v>1</v>
+      </c>
+      <c r="D49" s="3">
+        <v>1</v>
+      </c>
+      <c r="E49" s="3">
+        <v>0</v>
+      </c>
+      <c r="F49" s="3">
+        <v>0</v>
+      </c>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+      <c r="I49" s="5"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" s="5"/>
+      <c r="B50" s="5">
+        <v>1</v>
+      </c>
+      <c r="C50" s="5">
+        <v>1</v>
+      </c>
+      <c r="D50" s="6">
+        <v>1</v>
+      </c>
+      <c r="E50" s="5">
+        <v>0</v>
+      </c>
+      <c r="F50" s="5">
+        <v>1</v>
+      </c>
+      <c r="G50" s="5">
+        <v>0</v>
+      </c>
+      <c r="H50" s="5">
+        <v>0</v>
+      </c>
+      <c r="I50" s="5"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" s="5"/>
+      <c r="B51" s="3">
+        <v>1</v>
+      </c>
+      <c r="C51" s="3">
+        <v>1</v>
+      </c>
+      <c r="D51" s="3">
+        <v>1</v>
+      </c>
+      <c r="E51" s="3">
+        <v>1</v>
+      </c>
+      <c r="F51" s="3">
+        <v>0</v>
+      </c>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="5"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52" s="5"/>
+      <c r="B52" s="3">
+        <v>1</v>
+      </c>
+      <c r="C52" s="3">
+        <v>1</v>
+      </c>
+      <c r="D52" s="3">
+        <v>1</v>
+      </c>
+      <c r="E52" s="3">
+        <v>1</v>
+      </c>
+      <c r="F52" s="3">
+        <v>1</v>
+      </c>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="5"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53" s="5"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="9"/>
+      <c r="G53" s="9"/>
+      <c r="H53" s="9"/>
+      <c r="I53" s="9"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A54" s="5"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="9"/>
+      <c r="G54" s="9"/>
+      <c r="H54" s="9"/>
+      <c r="I54" s="9"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A55" s="5"/>
+      <c r="B55" s="5"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="10"/>
+      <c r="F55" s="10"/>
+      <c r="G55" s="10"/>
+      <c r="H55" s="9"/>
+      <c r="I55" s="9"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B56" s="5"/>
+      <c r="C56" s="11"/>
+      <c r="D56" s="11"/>
+      <c r="E56" s="11"/>
+      <c r="F56" s="11"/>
+      <c r="G56" s="11"/>
+      <c r="H56" s="9"/>
+      <c r="I56" s="12"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B57" s="5"/>
+      <c r="C57" s="11"/>
+      <c r="D57" s="11"/>
+      <c r="E57" s="11"/>
+      <c r="F57" s="11"/>
+      <c r="G57" s="11"/>
+      <c r="H57" s="9"/>
+      <c r="I57" s="12"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B58" s="5"/>
+      <c r="C58" s="11"/>
+      <c r="D58" s="11"/>
+      <c r="E58" s="11"/>
+      <c r="F58" s="11"/>
+      <c r="G58" s="11"/>
+      <c r="H58" s="9"/>
+      <c r="I58" s="12"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B59" s="5"/>
+      <c r="C59" s="11"/>
+      <c r="D59" s="11"/>
+      <c r="E59" s="11"/>
+      <c r="F59" s="11"/>
+      <c r="G59" s="11"/>
+      <c r="H59" s="9"/>
+      <c r="I59" s="12"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B60" s="5"/>
+      <c r="C60" s="11"/>
+      <c r="D60" s="11"/>
+      <c r="E60" s="11"/>
+      <c r="F60" s="11"/>
+      <c r="G60" s="11"/>
+      <c r="H60" s="9"/>
+      <c r="I60" s="12"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B61" s="5"/>
+      <c r="C61" s="11"/>
+      <c r="D61" s="11"/>
+      <c r="E61" s="11"/>
+      <c r="F61" s="11"/>
+      <c r="G61" s="11"/>
+      <c r="H61" s="9"/>
+      <c r="I61" s="12"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B62" s="5"/>
+      <c r="C62" s="11"/>
+      <c r="D62" s="11"/>
+      <c r="E62" s="11"/>
+      <c r="F62" s="11"/>
+      <c r="G62" s="11"/>
+      <c r="H62" s="9"/>
+      <c r="I62" s="12"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B63" s="5"/>
+      <c r="C63" s="11"/>
+      <c r="D63" s="11"/>
+      <c r="E63" s="11"/>
+      <c r="F63" s="11"/>
+      <c r="G63" s="11"/>
+      <c r="H63" s="9"/>
+      <c r="I63" s="12"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B64" s="5"/>
+      <c r="C64" s="11"/>
+      <c r="D64" s="11"/>
+      <c r="E64" s="11"/>
+      <c r="F64" s="11"/>
+      <c r="G64" s="11"/>
+      <c r="H64" s="9"/>
+      <c r="I64" s="12"/>
+    </row>
+    <row r="65" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B65" s="5"/>
+      <c r="C65" s="11"/>
+      <c r="D65" s="11"/>
+      <c r="E65" s="11"/>
+      <c r="F65" s="11"/>
+      <c r="G65" s="11"/>
+      <c r="H65" s="9"/>
+      <c r="I65" s="12"/>
+    </row>
+    <row r="66" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B66" s="9"/>
+      <c r="C66" s="11"/>
+      <c r="D66" s="11"/>
+      <c r="E66" s="11"/>
+      <c r="F66" s="11"/>
+      <c r="G66" s="11"/>
+      <c r="H66" s="9"/>
+      <c r="I66" s="12"/>
+    </row>
+    <row r="67" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B67" s="9"/>
+      <c r="C67" s="11"/>
+      <c r="D67" s="11"/>
+      <c r="E67" s="11"/>
+      <c r="F67" s="11"/>
+      <c r="G67" s="11"/>
+      <c r="H67" s="9"/>
+      <c r="I67" s="12"/>
+    </row>
+    <row r="68" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B68" s="9"/>
+      <c r="C68" s="11"/>
+      <c r="D68" s="11"/>
+      <c r="E68" s="11"/>
+      <c r="F68" s="11"/>
+      <c r="G68" s="11"/>
+      <c r="H68" s="9"/>
+    </row>
+    <row r="69" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B69" s="9"/>
+      <c r="C69" s="11"/>
+      <c r="D69" s="11"/>
+      <c r="E69" s="11"/>
+      <c r="F69" s="11"/>
+      <c r="G69" s="11"/>
+      <c r="H69" s="9"/>
+    </row>
+    <row r="70" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B70" s="9"/>
+      <c r="C70" s="11"/>
+      <c r="D70" s="11"/>
+      <c r="E70" s="11"/>
+      <c r="F70" s="11"/>
+      <c r="G70" s="11"/>
+      <c r="H70" s="9"/>
+    </row>
+    <row r="71" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B71" s="9"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="11"/>
+      <c r="E71" s="11"/>
+      <c r="F71" s="11"/>
+      <c r="G71" s="11"/>
+      <c r="H71" s="9"/>
+    </row>
+    <row r="72" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B72" s="9"/>
+      <c r="C72" s="11"/>
+      <c r="D72" s="11"/>
+      <c r="E72" s="11"/>
+      <c r="F72" s="11"/>
+      <c r="G72" s="11"/>
+      <c r="H72" s="9"/>
+    </row>
+    <row r="73" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B73" s="9"/>
+      <c r="C73" s="11"/>
+      <c r="D73" s="11"/>
+      <c r="E73" s="11"/>
+      <c r="F73" s="11"/>
+      <c r="G73" s="11"/>
+      <c r="H73" s="9"/>
+    </row>
+    <row r="74" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B74" s="9"/>
+      <c r="C74" s="11"/>
+      <c r="D74" s="11"/>
+      <c r="E74" s="11"/>
+      <c r="F74" s="11"/>
+      <c r="G74" s="11"/>
+      <c r="H74" s="9"/>
+    </row>
+    <row r="75" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B75" s="9"/>
+      <c r="C75" s="11"/>
+      <c r="D75" s="11"/>
+      <c r="E75" s="11"/>
+      <c r="F75" s="11"/>
+      <c r="G75" s="11"/>
+      <c r="H75" s="9"/>
+    </row>
+    <row r="76" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B76" s="9"/>
+      <c r="C76" s="11"/>
+      <c r="D76" s="11"/>
+      <c r="E76" s="11"/>
+      <c r="F76" s="11"/>
+      <c r="G76" s="11"/>
+      <c r="H76" s="9"/>
+    </row>
+    <row r="77" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B77" s="9"/>
+      <c r="C77" s="11"/>
+      <c r="D77" s="11"/>
+      <c r="E77" s="11"/>
+      <c r="F77" s="11"/>
+      <c r="G77" s="11"/>
+      <c r="H77" s="9"/>
+    </row>
+    <row r="78" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B78" s="9"/>
+      <c r="C78" s="11"/>
+      <c r="D78" s="11"/>
+      <c r="E78" s="11"/>
+      <c r="F78" s="11"/>
+      <c r="G78" s="11"/>
+      <c r="H78" s="9"/>
+    </row>
+    <row r="79" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B79" s="9"/>
+      <c r="C79" s="11"/>
+      <c r="D79" s="11"/>
+      <c r="E79" s="11"/>
+      <c r="F79" s="11"/>
+      <c r="G79" s="11"/>
+      <c r="H79" s="9"/>
+    </row>
+    <row r="80" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B80" s="9"/>
+      <c r="C80" s="11"/>
+      <c r="D80" s="11"/>
+      <c r="E80" s="11"/>
+      <c r="F80" s="11"/>
+      <c r="G80" s="11"/>
+      <c r="H80" s="9"/>
+    </row>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B81" s="9"/>
+      <c r="C81" s="11"/>
+      <c r="D81" s="11"/>
+      <c r="E81" s="11"/>
+      <c r="F81" s="11"/>
+      <c r="G81" s="11"/>
+      <c r="H81" s="9"/>
+    </row>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B82" s="9"/>
+      <c r="C82" s="11"/>
+      <c r="D82" s="11"/>
+      <c r="E82" s="11"/>
+      <c r="F82" s="11"/>
+      <c r="G82" s="11"/>
+      <c r="H82" s="9"/>
+    </row>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B83" s="5"/>
+      <c r="C83" s="11"/>
+      <c r="D83" s="11"/>
+      <c r="E83" s="11"/>
+      <c r="F83" s="11"/>
+      <c r="G83" s="11"/>
+      <c r="H83" s="9"/>
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B84" s="5"/>
+      <c r="C84" s="11"/>
+      <c r="D84" s="11"/>
+      <c r="E84" s="11"/>
+      <c r="F84" s="11"/>
+      <c r="G84" s="11"/>
+      <c r="H84" s="9"/>
+    </row>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B85" s="5"/>
+      <c r="C85" s="11"/>
+      <c r="D85" s="11"/>
+      <c r="E85" s="11"/>
+      <c r="F85" s="11"/>
+      <c r="G85" s="11"/>
+      <c r="H85" s="9"/>
+    </row>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B86" s="5"/>
+      <c r="C86" s="11"/>
+      <c r="D86" s="11"/>
+      <c r="E86" s="11"/>
+      <c r="F86" s="11"/>
+      <c r="G86" s="11"/>
+      <c r="H86" s="9"/>
+    </row>
+    <row r="87" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B87" s="5"/>
+      <c r="C87" s="11"/>
+      <c r="D87" s="11"/>
+      <c r="E87" s="11"/>
+      <c r="F87" s="11"/>
+      <c r="G87" s="11"/>
+      <c r="H87" s="9"/>
+    </row>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B88" s="5"/>
+      <c r="C88" s="5"/>
+      <c r="D88" s="5"/>
+      <c r="E88" s="5"/>
+      <c r="F88" s="5"/>
+      <c r="G88" s="5"/>
+      <c r="H88" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="F17 F2:F16" calculatedColumn="1"/>
   </ignoredErrors>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fatte alcune modifiche ai file
</commit_message>
<xml_diff>
--- a/input_signal_table.xlsx
+++ b/input_signal_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carloradice\Documents\IILTSpice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52911251-9614-42A6-A1AE-793E7339D096}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF551C6B-9A44-46FD-A603-AF57FF960E0C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -540,8 +540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J59" sqref="J59"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>